<commit_message>
adicionado coluna de referencia de regiao no Ox
</commit_message>
<xml_diff>
--- a/Database/GVAR Data/Dicionario.xlsx
+++ b/Database/GVAR Data/Dicionario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teo\Documents\Git\Tese\Database\GVAR Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{736E65D3-ED5E-41BE-B2FB-F20B4B42B1BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1398CC-AC94-491C-AE30-B02E50076A78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D79E37F2-CEE1-46C7-AA8E-2D8A0D111289}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="415">
   <si>
     <t>Name</t>
   </si>
@@ -864,6 +864,420 @@
   </si>
   <si>
     <t>Go5301</t>
+  </si>
+  <si>
+    <t>Ox</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>R36</t>
+  </si>
+  <si>
+    <t>R37</t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t>R39</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>R41</t>
+  </si>
+  <si>
+    <t>R42</t>
+  </si>
+  <si>
+    <t>R43</t>
+  </si>
+  <si>
+    <t>R44</t>
+  </si>
+  <si>
+    <t>R45</t>
+  </si>
+  <si>
+    <t>R46</t>
+  </si>
+  <si>
+    <t>R47</t>
+  </si>
+  <si>
+    <t>R48</t>
+  </si>
+  <si>
+    <t>R49</t>
+  </si>
+  <si>
+    <t>R50</t>
+  </si>
+  <si>
+    <t>R51</t>
+  </si>
+  <si>
+    <t>R52</t>
+  </si>
+  <si>
+    <t>R53</t>
+  </si>
+  <si>
+    <t>R54</t>
+  </si>
+  <si>
+    <t>R55</t>
+  </si>
+  <si>
+    <t>R56</t>
+  </si>
+  <si>
+    <t>R57</t>
+  </si>
+  <si>
+    <t>R58</t>
+  </si>
+  <si>
+    <t>R59</t>
+  </si>
+  <si>
+    <t>R60</t>
+  </si>
+  <si>
+    <t>R61</t>
+  </si>
+  <si>
+    <t>R62</t>
+  </si>
+  <si>
+    <t>R63</t>
+  </si>
+  <si>
+    <t>R64</t>
+  </si>
+  <si>
+    <t>R65</t>
+  </si>
+  <si>
+    <t>R66</t>
+  </si>
+  <si>
+    <t>R67</t>
+  </si>
+  <si>
+    <t>R68</t>
+  </si>
+  <si>
+    <t>R69</t>
+  </si>
+  <si>
+    <t>R70</t>
+  </si>
+  <si>
+    <t>R71</t>
+  </si>
+  <si>
+    <t>R72</t>
+  </si>
+  <si>
+    <t>R73</t>
+  </si>
+  <si>
+    <t>R74</t>
+  </si>
+  <si>
+    <t>R75</t>
+  </si>
+  <si>
+    <t>R76</t>
+  </si>
+  <si>
+    <t>R77</t>
+  </si>
+  <si>
+    <t>R78</t>
+  </si>
+  <si>
+    <t>R79</t>
+  </si>
+  <si>
+    <t>R80</t>
+  </si>
+  <si>
+    <t>R81</t>
+  </si>
+  <si>
+    <t>R82</t>
+  </si>
+  <si>
+    <t>R83</t>
+  </si>
+  <si>
+    <t>R84</t>
+  </si>
+  <si>
+    <t>R85</t>
+  </si>
+  <si>
+    <t>R86</t>
+  </si>
+  <si>
+    <t>R87</t>
+  </si>
+  <si>
+    <t>R88</t>
+  </si>
+  <si>
+    <t>R89</t>
+  </si>
+  <si>
+    <t>R90</t>
+  </si>
+  <si>
+    <t>R91</t>
+  </si>
+  <si>
+    <t>R92</t>
+  </si>
+  <si>
+    <t>R93</t>
+  </si>
+  <si>
+    <t>R94</t>
+  </si>
+  <si>
+    <t>R95</t>
+  </si>
+  <si>
+    <t>R96</t>
+  </si>
+  <si>
+    <t>R97</t>
+  </si>
+  <si>
+    <t>R98</t>
+  </si>
+  <si>
+    <t>R99</t>
+  </si>
+  <si>
+    <t>R100</t>
+  </si>
+  <si>
+    <t>R101</t>
+  </si>
+  <si>
+    <t>R102</t>
+  </si>
+  <si>
+    <t>R103</t>
+  </si>
+  <si>
+    <t>R104</t>
+  </si>
+  <si>
+    <t>R105</t>
+  </si>
+  <si>
+    <t>R106</t>
+  </si>
+  <si>
+    <t>R107</t>
+  </si>
+  <si>
+    <t>R108</t>
+  </si>
+  <si>
+    <t>R109</t>
+  </si>
+  <si>
+    <t>R110</t>
+  </si>
+  <si>
+    <t>R111</t>
+  </si>
+  <si>
+    <t>R112</t>
+  </si>
+  <si>
+    <t>R113</t>
+  </si>
+  <si>
+    <t>R114</t>
+  </si>
+  <si>
+    <t>R115</t>
+  </si>
+  <si>
+    <t>R116</t>
+  </si>
+  <si>
+    <t>R117</t>
+  </si>
+  <si>
+    <t>R118</t>
+  </si>
+  <si>
+    <t>R119</t>
+  </si>
+  <si>
+    <t>R120</t>
+  </si>
+  <si>
+    <t>R121</t>
+  </si>
+  <si>
+    <t>R122</t>
+  </si>
+  <si>
+    <t>R123</t>
+  </si>
+  <si>
+    <t>R124</t>
+  </si>
+  <si>
+    <t>R125</t>
+  </si>
+  <si>
+    <t>R126</t>
+  </si>
+  <si>
+    <t>R127</t>
+  </si>
+  <si>
+    <t>R128</t>
+  </si>
+  <si>
+    <t>R129</t>
+  </si>
+  <si>
+    <t>R130</t>
+  </si>
+  <si>
+    <t>R131</t>
+  </si>
+  <si>
+    <t>R132</t>
+  </si>
+  <si>
+    <t>R133</t>
+  </si>
+  <si>
+    <t>R134</t>
+  </si>
+  <si>
+    <t>R135</t>
+  </si>
+  <si>
+    <t>R136</t>
+  </si>
+  <si>
+    <t>R137</t>
   </si>
 </sst>
 </file>
@@ -1215,19 +1629,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5931D9DE-2CC2-45E8-B40B-46FDA6AF9941}">
-  <dimension ref="A1:C138"/>
+  <dimension ref="A1:D138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1237,8 +1652,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1248,8 +1666,11 @@
       <c r="C2">
         <v>1101</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1259,8 +1680,11 @@
       <c r="C3">
         <v>1102</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1270,8 +1694,11 @@
       <c r="C4">
         <v>1201</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1281,8 +1708,11 @@
       <c r="C5">
         <v>1202</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1292,8 +1722,11 @@
       <c r="C6">
         <v>1301</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1303,8 +1736,11 @@
       <c r="C7">
         <v>1302</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1314,8 +1750,11 @@
       <c r="C8">
         <v>1303</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1325,8 +1764,11 @@
       <c r="C9">
         <v>1304</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1336,8 +1778,11 @@
       <c r="C10">
         <v>1401</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1347,8 +1792,11 @@
       <c r="C11">
         <v>1402</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1358,8 +1806,11 @@
       <c r="C12">
         <v>1501</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1369,8 +1820,11 @@
       <c r="C13">
         <v>1502</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1380,8 +1834,11 @@
       <c r="C14">
         <v>1503</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1391,8 +1848,11 @@
       <c r="C15">
         <v>1504</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1402,8 +1862,11 @@
       <c r="C16">
         <v>1505</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1413,8 +1876,11 @@
       <c r="C17">
         <v>1506</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1424,8 +1890,11 @@
       <c r="C18">
         <v>1601</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1435,8 +1904,11 @@
       <c r="C19">
         <v>1602</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1446,8 +1918,11 @@
       <c r="C20">
         <v>1701</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1457,8 +1932,11 @@
       <c r="C21">
         <v>1702</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1468,8 +1946,11 @@
       <c r="C22">
         <v>2101</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1479,8 +1960,11 @@
       <c r="C23">
         <v>2102</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1490,8 +1974,11 @@
       <c r="C24">
         <v>2103</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -1501,8 +1988,11 @@
       <c r="C25">
         <v>2104</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1512,8 +2002,11 @@
       <c r="C26">
         <v>2105</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -1523,8 +2016,11 @@
       <c r="C27">
         <v>2201</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -1534,8 +2030,11 @@
       <c r="C28">
         <v>2202</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -1545,8 +2044,11 @@
       <c r="C29">
         <v>2203</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -1556,8 +2058,11 @@
       <c r="C30">
         <v>2204</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -1567,8 +2072,11 @@
       <c r="C31">
         <v>2301</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -1578,8 +2086,11 @@
       <c r="C32">
         <v>2302</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -1589,8 +2100,11 @@
       <c r="C33">
         <v>2303</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -1600,8 +2114,11 @@
       <c r="C34">
         <v>2304</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -1611,8 +2128,11 @@
       <c r="C35">
         <v>2305</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -1622,8 +2142,11 @@
       <c r="C36">
         <v>2306</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>73</v>
       </c>
@@ -1633,8 +2156,11 @@
       <c r="C37">
         <v>2307</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -1644,8 +2170,11 @@
       <c r="C38">
         <v>2401</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -1655,8 +2184,11 @@
       <c r="C39">
         <v>2402</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -1666,8 +2198,11 @@
       <c r="C40">
         <v>2403</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>81</v>
       </c>
@@ -1677,8 +2212,11 @@
       <c r="C41">
         <v>2404</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -1688,8 +2226,11 @@
       <c r="C42">
         <v>2501</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -1699,8 +2240,11 @@
       <c r="C43">
         <v>2502</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -1710,8 +2254,11 @@
       <c r="C44">
         <v>2503</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -1721,8 +2268,11 @@
       <c r="C45">
         <v>2504</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>91</v>
       </c>
@@ -1732,8 +2282,11 @@
       <c r="C46">
         <v>2601</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>93</v>
       </c>
@@ -1743,8 +2296,11 @@
       <c r="C47">
         <v>2602</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>95</v>
       </c>
@@ -1754,8 +2310,11 @@
       <c r="C48">
         <v>2603</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -1765,8 +2324,11 @@
       <c r="C49">
         <v>2604</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>99</v>
       </c>
@@ -1776,8 +2338,11 @@
       <c r="C50">
         <v>2605</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>101</v>
       </c>
@@ -1787,8 +2352,11 @@
       <c r="C51">
         <v>2701</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>103</v>
       </c>
@@ -1798,8 +2366,11 @@
       <c r="C52">
         <v>2702</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>105</v>
       </c>
@@ -1809,8 +2380,11 @@
       <c r="C53">
         <v>2703</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>107</v>
       </c>
@@ -1820,8 +2394,11 @@
       <c r="C54">
         <v>2801</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>109</v>
       </c>
@@ -1831,8 +2408,11 @@
       <c r="C55">
         <v>2802</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>111</v>
       </c>
@@ -1842,8 +2422,11 @@
       <c r="C56">
         <v>2803</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>113</v>
       </c>
@@ -1853,8 +2436,11 @@
       <c r="C57">
         <v>2901</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>115</v>
       </c>
@@ -1864,8 +2450,11 @@
       <c r="C58">
         <v>2902</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D58" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>117</v>
       </c>
@@ -1875,8 +2464,11 @@
       <c r="C59">
         <v>2903</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>119</v>
       </c>
@@ -1886,8 +2478,11 @@
       <c r="C60">
         <v>2904</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>121</v>
       </c>
@@ -1897,8 +2492,11 @@
       <c r="C61">
         <v>2905</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D61" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>123</v>
       </c>
@@ -1908,8 +2506,11 @@
       <c r="C62">
         <v>2906</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D62" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>125</v>
       </c>
@@ -1919,8 +2520,11 @@
       <c r="C63">
         <v>2907</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>127</v>
       </c>
@@ -1930,8 +2534,11 @@
       <c r="C64">
         <v>3101</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>129</v>
       </c>
@@ -1941,8 +2548,11 @@
       <c r="C65">
         <v>3102</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>131</v>
       </c>
@@ -1952,8 +2562,11 @@
       <c r="C66">
         <v>3103</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>133</v>
       </c>
@@ -1963,8 +2576,11 @@
       <c r="C67">
         <v>3104</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>135</v>
       </c>
@@ -1974,8 +2590,11 @@
       <c r="C68">
         <v>3105</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D68" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>137</v>
       </c>
@@ -1985,8 +2604,11 @@
       <c r="C69">
         <v>3106</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D69" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>139</v>
       </c>
@@ -1996,8 +2618,11 @@
       <c r="C70">
         <v>3107</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D70" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>141</v>
       </c>
@@ -2007,8 +2632,11 @@
       <c r="C71">
         <v>3108</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D71" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>143</v>
       </c>
@@ -2018,8 +2646,11 @@
       <c r="C72">
         <v>3109</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D72" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>145</v>
       </c>
@@ -2029,8 +2660,11 @@
       <c r="C73">
         <v>3110</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D73" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>147</v>
       </c>
@@ -2040,8 +2674,11 @@
       <c r="C74">
         <v>3111</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D74" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>149</v>
       </c>
@@ -2051,8 +2688,11 @@
       <c r="C75">
         <v>3112</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>151</v>
       </c>
@@ -2062,8 +2702,11 @@
       <c r="C76">
         <v>3201</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D76" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>153</v>
       </c>
@@ -2073,8 +2716,11 @@
       <c r="C77">
         <v>3202</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D77" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>155</v>
       </c>
@@ -2084,8 +2730,11 @@
       <c r="C78">
         <v>3203</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D78" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>157</v>
       </c>
@@ -2095,8 +2744,11 @@
       <c r="C79">
         <v>3204</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D79" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>159</v>
       </c>
@@ -2106,8 +2758,11 @@
       <c r="C80">
         <v>3301</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>161</v>
       </c>
@@ -2117,8 +2772,11 @@
       <c r="C81">
         <v>3302</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>163</v>
       </c>
@@ -2128,8 +2786,11 @@
       <c r="C82">
         <v>3303</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>165</v>
       </c>
@@ -2139,8 +2800,11 @@
       <c r="C83">
         <v>3304</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D83" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>167</v>
       </c>
@@ -2150,8 +2814,11 @@
       <c r="C84">
         <v>3305</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D84" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>169</v>
       </c>
@@ -2161,8 +2828,11 @@
       <c r="C85">
         <v>3306</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D85" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>171</v>
       </c>
@@ -2172,8 +2842,11 @@
       <c r="C86">
         <v>3501</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D86" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>173</v>
       </c>
@@ -2183,8 +2856,11 @@
       <c r="C87">
         <v>3502</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D87" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>175</v>
       </c>
@@ -2194,8 +2870,11 @@
       <c r="C88">
         <v>3503</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D88" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>177</v>
       </c>
@@ -2205,8 +2884,11 @@
       <c r="C89">
         <v>3504</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D89" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>179</v>
       </c>
@@ -2216,8 +2898,11 @@
       <c r="C90">
         <v>3505</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D90" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>181</v>
       </c>
@@ -2227,8 +2912,11 @@
       <c r="C91">
         <v>3506</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D91" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>183</v>
       </c>
@@ -2238,8 +2926,11 @@
       <c r="C92">
         <v>3507</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D92" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>185</v>
       </c>
@@ -2249,8 +2940,11 @@
       <c r="C93">
         <v>3508</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D93" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>187</v>
       </c>
@@ -2260,8 +2954,11 @@
       <c r="C94">
         <v>3509</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D94" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>189</v>
       </c>
@@ -2271,8 +2968,11 @@
       <c r="C95">
         <v>3510</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D95" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>191</v>
       </c>
@@ -2282,8 +2982,11 @@
       <c r="C96">
         <v>3511</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D96" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>193</v>
       </c>
@@ -2293,8 +2996,11 @@
       <c r="C97">
         <v>3512</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D97" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>195</v>
       </c>
@@ -2304,8 +3010,11 @@
       <c r="C98">
         <v>3513</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D98" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>197</v>
       </c>
@@ -2315,8 +3024,11 @@
       <c r="C99">
         <v>3514</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D99" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>199</v>
       </c>
@@ -2326,8 +3038,11 @@
       <c r="C100">
         <v>3515</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D100" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>201</v>
       </c>
@@ -2337,8 +3052,11 @@
       <c r="C101">
         <v>4101</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D101" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>203</v>
       </c>
@@ -2348,8 +3066,11 @@
       <c r="C102">
         <v>4102</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D102" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>205</v>
       </c>
@@ -2359,8 +3080,11 @@
       <c r="C103">
         <v>4103</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D103" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>207</v>
       </c>
@@ -2370,8 +3094,11 @@
       <c r="C104">
         <v>4104</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D104" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>209</v>
       </c>
@@ -2381,8 +3108,11 @@
       <c r="C105">
         <v>4105</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D105" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>211</v>
       </c>
@@ -2392,8 +3122,11 @@
       <c r="C106">
         <v>4106</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D106" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>213</v>
       </c>
@@ -2403,8 +3136,11 @@
       <c r="C107">
         <v>4107</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D107" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>215</v>
       </c>
@@ -2414,8 +3150,11 @@
       <c r="C108">
         <v>4108</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D108" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>217</v>
       </c>
@@ -2425,8 +3164,11 @@
       <c r="C109">
         <v>4109</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D109" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>219</v>
       </c>
@@ -2436,8 +3178,11 @@
       <c r="C110">
         <v>4110</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D110" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>221</v>
       </c>
@@ -2447,8 +3192,11 @@
       <c r="C111">
         <v>4201</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D111" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>223</v>
       </c>
@@ -2458,8 +3206,11 @@
       <c r="C112">
         <v>4202</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D112" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>225</v>
       </c>
@@ -2469,8 +3220,11 @@
       <c r="C113">
         <v>4203</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D113" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>227</v>
       </c>
@@ -2480,8 +3234,11 @@
       <c r="C114">
         <v>4204</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D114" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>229</v>
       </c>
@@ -2491,8 +3248,11 @@
       <c r="C115">
         <v>4205</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D115" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>231</v>
       </c>
@@ -2502,8 +3262,11 @@
       <c r="C116">
         <v>4206</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D116" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>233</v>
       </c>
@@ -2513,8 +3276,11 @@
       <c r="C117">
         <v>4301</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D117" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>235</v>
       </c>
@@ -2524,8 +3290,11 @@
       <c r="C118">
         <v>4302</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D118" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>237</v>
       </c>
@@ -2535,8 +3304,11 @@
       <c r="C119">
         <v>4303</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D119" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>239</v>
       </c>
@@ -2546,8 +3318,11 @@
       <c r="C120">
         <v>4304</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D120" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>241</v>
       </c>
@@ -2557,8 +3332,11 @@
       <c r="C121">
         <v>4305</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D121" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>243</v>
       </c>
@@ -2568,8 +3346,11 @@
       <c r="C122">
         <v>4306</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D122" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>245</v>
       </c>
@@ -2579,8 +3360,11 @@
       <c r="C123">
         <v>4307</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D123" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>247</v>
       </c>
@@ -2590,8 +3374,11 @@
       <c r="C124">
         <v>5001</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D124" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>249</v>
       </c>
@@ -2601,8 +3388,11 @@
       <c r="C125">
         <v>5002</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D125" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>251</v>
       </c>
@@ -2612,8 +3402,11 @@
       <c r="C126">
         <v>5003</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D126" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>253</v>
       </c>
@@ -2623,8 +3416,11 @@
       <c r="C127">
         <v>5004</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D127" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>255</v>
       </c>
@@ -2634,8 +3430,11 @@
       <c r="C128">
         <v>5101</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D128" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>257</v>
       </c>
@@ -2645,8 +3444,11 @@
       <c r="C129">
         <v>5102</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D129" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>259</v>
       </c>
@@ -2656,8 +3458,11 @@
       <c r="C130">
         <v>5103</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D130" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>261</v>
       </c>
@@ -2667,8 +3472,11 @@
       <c r="C131">
         <v>5104</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D131" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>263</v>
       </c>
@@ -2678,8 +3486,11 @@
       <c r="C132">
         <v>5105</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D132" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>265</v>
       </c>
@@ -2689,8 +3500,11 @@
       <c r="C133">
         <v>5201</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D133" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>267</v>
       </c>
@@ -2700,8 +3514,11 @@
       <c r="C134">
         <v>5202</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D134" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>269</v>
       </c>
@@ -2711,8 +3528,11 @@
       <c r="C135">
         <v>5203</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D135" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>271</v>
       </c>
@@ -2722,8 +3542,11 @@
       <c r="C136">
         <v>5204</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D136" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>273</v>
       </c>
@@ -2733,8 +3556,11 @@
       <c r="C137">
         <v>5205</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D137" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>275</v>
       </c>
@@ -2743,6 +3569,9 @@
       </c>
       <c r="C138">
         <v>5301</v>
+      </c>
+      <c r="D138" t="s">
+        <v>414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>